<commit_message>
updating github with pull / push of recent edits/deletions of .py files
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,12 +434,34 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Italian</t>
+          <t>Finnish</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
           <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>129° - Weetabix cereal 48 pack £3.50 at Asda</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Finnish</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>129 ° - Weetabix-muroja 48 kpl 3,50 puntaa Asdassa</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.hotukdeals.com/deals/rollback-ps350-weetabix-cereal-at-asda-3571010</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
creating a requirements.txt file for virtual environment setup
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Finnish</t>
+          <t>Danish</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -446,22 +446,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>129° - Weetabix cereal 48 pack £3.50 at Asda</t>
+          <t>UK will ban mobile carriers from selling locked handsets in 2021</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Finnish</t>
+          <t>Danish</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>129 ° - Weetabix-muroja 48 kpl 3,50 puntaa Asdassa</t>
+          <t>Storbritannien forbyder mobiloperatører at sælge låste håndsæt i 2021</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.hotukdeals.com/deals/rollback-ps350-weetabix-cereal-at-asda-3571010</t>
+          <t>https://www.engadget.com/uk-bans-mobile-companies-from-selling-locked-handsets-103533257.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tesco fast tracks emissions target with solar push - Reuters UK</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Danish</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tesco sporer hurtigt emissionsmål med solskub - Reuters UK</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://uk.reuters.com/article/uk-tesco-emissions-idUKKBN27T001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Asda, Tesco, Sainsbury's and Aldi warn shoppers what they can buy during second lockdown - Kent Live</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Danish</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Asda, Tesco, Sainsbury og Aldi advarer shoppere om, hvad de kan købe under anden lockdown - Kent Live</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.kentlive.news/whats-on/shopping/asda-tesco-sainsburys-aldi-warn-4680621</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
had to do many changes to original project as google translate had become unstable, had to fix way inverted commas were stripped before passing to mysql, copied over flask project from machine learning, and started prep work to adapt for this project
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,20 +424,10 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Headline Title</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
-        <is>
-          <t>Translation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Danish</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
@@ -446,66 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UK will ban mobile carriers from selling locked handsets in 2021</t>
+          <t>France starts collecting tax on tech giants</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Danish</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Storbritannien forbyder mobiloperatører at sælge låste håndsæt i 2021</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.engadget.com/uk-bans-mobile-companies-from-selling-locked-handsets-103533257.html</t>
+          <t>http://techcrunch.com/2020/11/25/france-starts-collecting-tax-on-tech-giants/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tesco fast tracks emissions target with solar push - Reuters UK</t>
+          <t>France to Tech Giants: Pay Up, Buttercup</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Danish</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tesco sporer hurtigt emissionsmål med solskub - Reuters UK</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://uk.reuters.com/article/uk-tesco-emissions-idUKKBN27T001</t>
+          <t>https://gizmodo.com/france-to-tech-giants-pay-up-buttercup-1845757236</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Asda, Tesco, Sainsbury's and Aldi warn shoppers what they can buy during second lockdown - Kent Live</t>
+          <t>Why France may ban discrimination against accents</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Danish</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Asda, Tesco, Sainsbury og Aldi advarer shoppere om, hvad de kan købe under anden lockdown - Kent Live</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://www.kentlive.news/whats-on/shopping/asda-tesco-sainsburys-aldi-warn-4680621</t>
+          <t>https://www.bbc.co.uk/news/world-europe-55069048</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Coronavirus: France replaces lockdown with evening curfew</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55324422</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>France police security bill: Protests turn violent again</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55201993</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Where Are Your Papers? A New Yorker Goes Home to Locked-Down France</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.nytimes.com/2020/12/10/us/france-lockdown-compare-new-york.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Patrick Vieira: Nice sack manager after two and a half years in charge</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/sport/football/55187481</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Covid: Students and retirees form long-distance friendships</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55235378</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Charlie Hebdo: Fourteen guilty in 2015 Paris terror attacks trial</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55336094</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trial of ex-president Sarkozy a landmark for France</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55015479</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>France Islam: Muslims face state pressure to embrace values</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55132098</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Radio France Internationale publishes obituaries of people still alive</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-54965098</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>France Islam: French cabinet backs law targeting extremism</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55253832</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Lockdowns Aren’t Funny. But You’ve Still Got to Laugh.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.nytimes.com/2020/11/19/theater/france-lockdown-comedy.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Obituary: Valéry Giscard DEstaing</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-13062449</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>French police seize 10 tigers after mistreatment complaint</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/world-europe-55337455</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>French rugby legend Dominici dies in park tragedy</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/news/55056643</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ireland and Scotland in same 2023 World Cup pool as South Africa</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/sport/rugby-union/55301480</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Man Citys Torres hits hat-trick as Spain put six past Germany to reach Nations League finals</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/sport/football/54979319</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wasps hooker Barbeary called up to England squad</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.bbc.co.uk/sport/rugby-union/55139252</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
It has been a while between commits, I've tried to repurpose some code from Machine Learning Assignment, I have also setup an online MySql account service, having some difficulty getting it to add to database, but can display database, also trying to integrate Matplotlib graphs into project
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>France starts collecting tax on tech giants</t>
+          <t>Is the New Visa Bitcoin Rewards Card Worth It?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/11/25/france-starts-collecting-tax-on-tech-giants/</t>
+          <t>https://twocents.lifehacker.com/is-the-new-visa-bitcoin-rewards-card-worth-it-1845803159</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>France to Tech Giants: Pay Up, Buttercup</t>
+          <t>Bitcoin passes $20k and reaches all-time high</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://gizmodo.com/france-to-tech-giants-pay-up-buttercup-1845757236</t>
+          <t>http://techcrunch.com/2020/12/16/bitcoin-passes-20k-and-reaches-all-time-high/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Why France may ban discrimination against accents</t>
+          <t>Bitcoin Blows Past $20,000 Milestone</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55069048</t>
+          <t>https://gizmodo.com/bitcoin-blows-past-20-000-milestone-1845894176</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Coronavirus: France replaces lockdown with evening curfew</t>
+          <t>Is rising usage driving crypto’s recent price boom?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55324422</t>
+          <t>http://techcrunch.com/2020/12/17/is-rising-usage-driving-cryptos-recent-price-boom/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>France police security bill: Protests turn violent again</t>
+          <t>Bitcoin is flirting with $20,000 again. How high will it go this time?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55201993</t>
+          <t>https://mashable.com/article/bitcoin-20000/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Where Are Your Papers? A New Yorker Goes Home to Locked-Down France</t>
+          <t>You can now spend Chinas digital currency at an online store</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/12/10/us/france-lockdown-compare-new-york.html</t>
+          <t>https://www.engadget.com/jd-com-supports-china-digital-currency-223718682.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Patrick Vieira: Nice sack manager after two and a half years in charge</t>
+          <t>Bitcoin Could Hit $20K Again But This Time No One Cares</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/sport/football/55187481</t>
+          <t>https://gizmodo.com/bitcoin-could-hit-20k-again-but-this-time-no-one-cares-1845757159</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Covid: Students and retirees form long-distance friendships</t>
+          <t>Bitcoin hits all-time high rising above $20,000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55235378</t>
+          <t>https://www.bbc.co.uk/news/business-55343657</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Charlie Hebdo: Fourteen guilty in 2015 Paris terror attacks trial</t>
+          <t>With investors expecting a Latin American cryptocurrency boom, Mexico’s Bitso raises $62 million</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55336094</t>
+          <t>http://techcrunch.com/2020/12/09/with-investors-expecting-a-latin-american-cryptocurrency-boom-mexicos-bitso-raises-62-million/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trial of ex-president Sarkozy a landmark for France</t>
+          <t>As Crypto comes back, Binance-backed Injective Protocol launches Testnet for its DeFi trading platform</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55015479</t>
+          <t>http://techcrunch.com/2020/12/03/as-crypto-comes-back-binance-backed-injective-protocol-launches-testnet-for-its-defi-trading-platform/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>France Islam: Muslims face state pressure to embrace values</t>
+          <t>Bitcoin soars after BlackRock says it could replace gold</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55132098</t>
+          <t>https://www.cnn.com/2020/11/20/investing/bitcoin-prices-gold-blackrock/index.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Radio France Internationale publishes obituaries of people still alive</t>
+          <t>Online Shopping, Virus in Winter, Stock Market: Your Monday Evening Briefing</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-54965098</t>
+          <t>https://www.nytimes.com/2020/11/30/briefing/online-shopping-virus-in-winter-stock-market.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>France Islam: French cabinet backs law targeting extremism</t>
+          <t>Months later, the great Twitter hack still boggles my mind</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55253832</t>
+          <t>https://www.theverge.com/22163643/twitter-hack-bitcoin-scam-july-2020-elon-musk</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lockdowns Aren’t Funny. But You’ve Still Got to Laugh.</t>
+          <t>Bitcoin price soars above $18,000, the highest level since 2017</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/11/19/theater/france-lockdown-comedy.html</t>
+          <t>https://arstechnica.com/tech-policy/2020/11/bitcoin-price-soars-above-18000-the-highest-level-since-2017/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Obituary: Valéry Giscard DEstaing</t>
+          <t>Bitcoin price passes $20,000, setting new record</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-13062449</t>
+          <t>https://arstechnica.com/tech-policy/2020/12/bitcoin-price-passes-20000-setting-new-record/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>French police seize 10 tigers after mistreatment complaint</t>
+          <t>Bitcoin breaks above $20,000 for first time - Reuters</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55337455</t>
+          <t>https://www.reuters.com/article/crypto-currency-idUSKBN28Q1UI</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>French rugby legend Dominici dies in park tragedy</t>
+          <t>Bitcoin breaks above $20,000 for first time - Reuters India</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/55056643</t>
+          <t>https://in.reuters.com/article/crypto-currency-idINKBN28Q1W8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ireland and Scotland in same 2023 World Cup pool as South Africa</t>
+          <t>Bitcoin hits nearly three-year peak, homes in on record - Reuters.com</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/sport/rugby-union/55301480</t>
+          <t>https://uk.reuters.com/article/us-crypto-currencies-idUSKBN27X2PQ</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Man Citys Torres hits hat-trick as Spain put six past Germany to reach Nations League finals</t>
+          <t>Cryptocurrency: Bitcoin hits three-year high as investors jump in - BBC News</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/sport/football/54979319</t>
+          <t>https://www.bbc.com/news/business-54982604</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Wasps hooker Barbeary called up to England squad</t>
+          <t>How American investors are buying bitcoin - Reuters.com</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/sport/rugby-union/55139252</t>
+          <t>https://www.reuters.com/video/watch/idOVD7GKP6Z</t>
         </is>
       </c>
     </row>

</xml_diff>